<commit_message>
Added url excel sheet. Changed TOC-> TableofContents
</commit_message>
<xml_diff>
--- a/URL_List/liburl.xlsx
+++ b/URL_List/liburl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChetanKanakeri\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChetanKanakeri\PycharmProjects\ibm-dotcom-library\URL_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86893CA-1BED-4161-980E-5505E68C9E5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C006748-74B8-4C2C-BDBD-12909AB581C1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>https://ibmdotcom-react-experimental.mybluemix.net/</t>
   </si>
   <si>
     <t>https://ibmdotcom-react-staging.mybluemix.net/</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit. Vivamus est purus, posuere at est vitae, ornare rhoncus sem. Suspendisse vitae tellus fermentum, hendrerit augue eu, placerat magna.Lorem ipsum dolor sit amet, consectetur adipiscing elit. Vivamus est purus, posuere at est vitae, ornare rhoncus sem. Suspendisse vitae tellus fermentum, hendrerit augue eu, placerat magna.Lorem ipsum dolor sit amet, consectetur adipiscing elit. Vivamus est purus, posuere at est vitae, ornare rhoncus sem. Suspendisse vitae tellus fermentum, hendrerit augue eu, placerat magna.</t>
   </si>
   <si>
     <t>https://ibmdotcom-react-canary.mybluemix.net/</t>
@@ -374,10 +371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,22 +384,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>